<commit_message>
remove excel tmp files
</commit_message>
<xml_diff>
--- a/Assets/Excels/全局设置表.xlsx
+++ b/Assets/Excels/全局设置表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A723BA34-9BF2-164A-80D5-FF9A772CAB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187C4B8E-7097-4947-B4E9-4FB6FEEDCB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,10 +230,6 @@
   </si>
   <si>
     <t>治疗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CardIcon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -427,6 +423,10 @@
   </si>
   <si>
     <t>合战场景配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CardIcon[]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -964,10 +964,10 @@
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="16">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16">
@@ -1177,7 +1177,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16">
@@ -1198,10 +1198,10 @@
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>58</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16">
@@ -1209,11 +1209,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16">
@@ -1221,11 +1221,11 @@
         <v>18</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16">
@@ -1305,11 +1305,11 @@
         <v>30</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16">
@@ -1318,10 +1318,10 @@
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17">
@@ -1329,11 +1329,11 @@
         <v>32</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1392,7 +1392,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16">
@@ -1546,7 +1546,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16">
@@ -1557,7 +1557,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16">
@@ -1568,7 +1568,7 @@
         <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16">
@@ -1579,7 +1579,7 @@
         <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16">
@@ -1590,7 +1590,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16">
@@ -1601,7 +1601,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16">
@@ -1612,7 +1612,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3">

</xml_diff>